<commit_message>
Translated notifications and Premission error handling.
</commit_message>
<xml_diff>
--- a/Lagerbestand-M0129.xlsx
+++ b/Lagerbestand-M0129.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2725</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2521</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="10">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D14" s="1" t="n">
-        <v>4948</v>
+        <v>4768</v>
       </c>
     </row>
     <row r="15">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D22" s="1" t="n">
-        <v>2038</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="23">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D29" s="1" t="n">
-        <v>6221</v>
+        <v>6017</v>
       </c>
     </row>
     <row r="30">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="D30" s="1" t="n">
-        <v>-181</v>
+        <v>-235</v>
       </c>
     </row>
     <row r="31">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="D33" s="1" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="D40" s="1" t="n">
-        <v>-17</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="41">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="D41" s="1" t="n">
-        <v>5677</v>
+        <v>5473</v>
       </c>
     </row>
     <row r="42">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D42" s="1" t="n">
-        <v>3975</v>
+        <v>3771</v>
       </c>
     </row>
     <row r="43">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="D43" s="1" t="n">
-        <v>388</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D45" s="1" t="n">
-        <v>3154</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="46">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="D46" s="1" t="n">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47">
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="D48" s="1" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49">
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="D51" s="1" t="n">
-        <v>-340</v>
+        <v>-400</v>
       </c>
     </row>
     <row r="52">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D52" s="1" t="n">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53">
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="D53" s="1" t="n">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1828</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="57">
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="D63" s="1" t="n">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D75" s="1" t="n">
-        <v>256</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="D76" s="1" t="n">
-        <v>4894</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="77">
@@ -1816,7 +1816,7 @@
         </is>
       </c>
       <c r="D82" s="1" t="n">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="D90" s="1" t="n">
-        <v>713</v>
+        <v>686</v>
       </c>
     </row>
     <row r="91">
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="D91" s="1" t="n">
-        <v>709</v>
+        <v>691</v>
       </c>
     </row>
     <row r="92">
@@ -1996,7 +1996,7 @@
         </is>
       </c>
       <c r="D92" s="1" t="n">
-        <v>869</v>
+        <v>857</v>
       </c>
     </row>
     <row r="93">
@@ -2014,7 +2014,7 @@
         </is>
       </c>
       <c r="D93" s="1" t="n">
-        <v>650</v>
+        <v>629</v>
       </c>
     </row>
     <row r="94">
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="D97" s="1" t="n">
-        <v>898</v>
+        <v>868</v>
       </c>
     </row>
     <row r="98">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="D99" s="1" t="n">
-        <v>487</v>
+        <v>463</v>
       </c>
     </row>
     <row r="100">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="D118" s="1" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="D124" s="1" t="n">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="125">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="D125" s="1" t="n">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="126">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="D127" s="1" t="n">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="128">
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="D155" s="1" t="n">
-        <v>2542</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="156">
@@ -3220,7 +3220,7 @@
         </is>
       </c>
       <c r="D160" s="1" t="n">
-        <v>723</v>
+        <v>702</v>
       </c>
     </row>
     <row r="161">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="D181" s="1" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="182">
@@ -3616,7 +3616,7 @@
         </is>
       </c>
       <c r="D182" s="1" t="n">
-        <v>-34</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="183">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="D207" s="1" t="n">
-        <v>-1707</v>
+        <v>-2008.5</v>
       </c>
     </row>
     <row r="208">
@@ -4390,7 +4390,7 @@
         </is>
       </c>
       <c r="D225" s="1" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="226">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="D230" s="1" t="n">
-        <v>-425</v>
+        <v>-500</v>
       </c>
     </row>
     <row r="231">
@@ -4498,7 +4498,7 @@
         </is>
       </c>
       <c r="D231" s="1" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="232">
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="D238" s="1" t="n">
-        <v>-1700</v>
+        <v>-2000</v>
       </c>
     </row>
     <row r="239">
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="D242" s="1" t="n">
-        <v>5</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="243">

</xml_diff>

<commit_message>
Splited common functions and config files + added name changing
</commit_message>
<xml_diff>
--- a/Lagerbestand-M0129.xlsx
+++ b/Lagerbestand-M0129.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2575</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2491</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="10">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D14" s="1" t="n">
-        <v>4768</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="15">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D22" s="1" t="n">
-        <v>2017</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="23">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D29" s="1" t="n">
-        <v>6017</v>
+        <v>3161</v>
       </c>
     </row>
     <row r="30">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="D30" s="1" t="n">
-        <v>-235</v>
+        <v>-991</v>
       </c>
     </row>
     <row r="31">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="D33" s="1" t="n">
-        <v>29</v>
+        <v>-97</v>
       </c>
     </row>
     <row r="34">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="D40" s="1" t="n">
-        <v>-20</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="41">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="D41" s="1" t="n">
-        <v>5473</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="42">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D42" s="1" t="n">
-        <v>3771</v>
+        <v>915</v>
       </c>
     </row>
     <row r="43">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="D43" s="1" t="n">
-        <v>232</v>
+        <v>-1952</v>
       </c>
     </row>
     <row r="44">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D45" s="1" t="n">
-        <v>3100</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="46">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="D46" s="1" t="n">
-        <v>151</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47">
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="D48" s="1" t="n">
-        <v>72</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="49">
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="D51" s="1" t="n">
-        <v>-400</v>
+        <v>-1240</v>
       </c>
     </row>
     <row r="52">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D52" s="1" t="n">
-        <v>244</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="53">
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="D53" s="1" t="n">
-        <v>196</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1786</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="57">
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="D63" s="1" t="n">
-        <v>47</v>
+        <v>-163</v>
       </c>
     </row>
     <row r="64">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D75" s="1" t="n">
-        <v>211</v>
+        <v>-419</v>
       </c>
     </row>
     <row r="76">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="D76" s="1" t="n">
-        <v>4594</v>
+        <v>394</v>
       </c>
     </row>
     <row r="77">
@@ -1816,7 +1816,7 @@
         </is>
       </c>
       <c r="D82" s="1" t="n">
-        <v>216</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="D90" s="1" t="n">
-        <v>686</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91">
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="D91" s="1" t="n">
-        <v>691</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92">
@@ -1996,7 +1996,7 @@
         </is>
       </c>
       <c r="D92" s="1" t="n">
-        <v>857</v>
+        <v>689</v>
       </c>
     </row>
     <row r="93">
@@ -2014,7 +2014,7 @@
         </is>
       </c>
       <c r="D93" s="1" t="n">
-        <v>629</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94">
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="D97" s="1" t="n">
-        <v>868</v>
+        <v>448</v>
       </c>
     </row>
     <row r="98">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="D99" s="1" t="n">
-        <v>463</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="D118" s="1" t="n">
-        <v>2</v>
+        <v>-166</v>
       </c>
     </row>
     <row r="119">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="D124" s="1" t="n">
-        <v>308</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="D125" s="1" t="n">
-        <v>62</v>
+        <v>-64</v>
       </c>
     </row>
     <row r="126">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="D127" s="1" t="n">
-        <v>403</v>
+        <v>361</v>
       </c>
     </row>
     <row r="128">
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="D155" s="1" t="n">
-        <v>2242</v>
+        <v>-1958</v>
       </c>
     </row>
     <row r="156">
@@ -3220,7 +3220,7 @@
         </is>
       </c>
       <c r="D160" s="1" t="n">
-        <v>702</v>
+        <v>408</v>
       </c>
     </row>
     <row r="161">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="D181" s="1" t="n">
-        <v>38</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="182">
@@ -3616,7 +3616,7 @@
         </is>
       </c>
       <c r="D182" s="1" t="n">
-        <v>-40</v>
+        <v>-124</v>
       </c>
     </row>
     <row r="183">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="D207" s="1" t="n">
-        <v>-2008.5</v>
+        <v>-6229</v>
       </c>
     </row>
     <row r="208">
@@ -4390,7 +4390,7 @@
         </is>
       </c>
       <c r="D225" s="1" t="n">
-        <v>42</v>
+        <v>-42</v>
       </c>
     </row>
     <row r="226">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="D230" s="1" t="n">
-        <v>-500</v>
+        <v>-1550</v>
       </c>
     </row>
     <row r="231">
@@ -4498,7 +4498,7 @@
         </is>
       </c>
       <c r="D231" s="1" t="n">
-        <v>20</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="232">
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="D238" s="1" t="n">
-        <v>-2000</v>
+        <v>-6200</v>
       </c>
     </row>
     <row r="239">
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="D242" s="1" t="n">
-        <v>-10</v>
+        <v>-220</v>
       </c>
     </row>
     <row r="243">

</xml_diff>

<commit_message>
added config file with unix path system
</commit_message>
<xml_diff>
--- a/Lagerbestand-M0129.xlsx
+++ b/Lagerbestand-M0129.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>325</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2041</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="10">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D14" s="1" t="n">
-        <v>2068</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="15">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D22" s="1" t="n">
-        <v>1702</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="23">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D29" s="1" t="n">
-        <v>2957</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="30">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="D30" s="1" t="n">
-        <v>-1045</v>
+        <v>-1063</v>
       </c>
     </row>
     <row r="31">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="D33" s="1" t="n">
-        <v>-106</v>
+        <v>-109</v>
       </c>
     </row>
     <row r="34">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="D40" s="1" t="n">
-        <v>-65</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="41">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="D41" s="1" t="n">
-        <v>2413</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="42">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D42" s="1" t="n">
-        <v>711</v>
+        <v>643</v>
       </c>
     </row>
     <row r="43">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="D43" s="1" t="n">
-        <v>-2108</v>
+        <v>-2160</v>
       </c>
     </row>
     <row r="44">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D45" s="1" t="n">
-        <v>2290</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="46">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="D46" s="1" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47">
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="D48" s="1" t="n">
-        <v>-18</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="49">
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="D51" s="1" t="n">
-        <v>-1300</v>
+        <v>-1320</v>
       </c>
     </row>
     <row r="52">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D52" s="1" t="n">
-        <v>-26</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="53">
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="D53" s="1" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1156</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="57">
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="D63" s="1" t="n">
-        <v>-178</v>
+        <v>-183</v>
       </c>
     </row>
     <row r="64">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D75" s="1" t="n">
-        <v>-464</v>
+        <v>-479</v>
       </c>
     </row>
     <row r="76">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="D76" s="1" t="n">
-        <v>94</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="77">
@@ -1816,7 +1816,7 @@
         </is>
       </c>
       <c r="D82" s="1" t="n">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="D90" s="1" t="n">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="91">
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="D91" s="1" t="n">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="92">
@@ -1996,7 +1996,7 @@
         </is>
       </c>
       <c r="D92" s="1" t="n">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="93">
@@ -2014,7 +2014,7 @@
         </is>
       </c>
       <c r="D93" s="1" t="n">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="94">
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="D97" s="1" t="n">
-        <v>418</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="D99" s="1" t="n">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="D118" s="1" t="n">
-        <v>-178</v>
+        <v>-182</v>
       </c>
     </row>
     <row r="119">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="D124" s="1" t="n">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="125">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="D125" s="1" t="n">
-        <v>-73</v>
+        <v>-76</v>
       </c>
     </row>
     <row r="126">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="D127" s="1" t="n">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="128">
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="D155" s="1" t="n">
-        <v>-2258</v>
+        <v>-2358</v>
       </c>
     </row>
     <row r="156">
@@ -3220,7 +3220,7 @@
         </is>
       </c>
       <c r="D160" s="1" t="n">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="161">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="D181" s="1" t="n">
-        <v>-52</v>
+        <v>-54</v>
       </c>
     </row>
     <row r="182">
@@ -3616,7 +3616,7 @@
         </is>
       </c>
       <c r="D182" s="1" t="n">
-        <v>-130</v>
+        <v>-132</v>
       </c>
     </row>
     <row r="183">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="D207" s="1" t="n">
-        <v>-6529</v>
+        <v>-6629</v>
       </c>
     </row>
     <row r="208">
@@ -4390,7 +4390,7 @@
         </is>
       </c>
       <c r="D225" s="1" t="n">
-        <v>-48</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="226">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="D230" s="1" t="n">
-        <v>-1625</v>
+        <v>-1650</v>
       </c>
     </row>
     <row r="231">
@@ -4498,7 +4498,7 @@
         </is>
       </c>
       <c r="D231" s="1" t="n">
-        <v>-25</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="232">
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="D238" s="1" t="n">
-        <v>-6500</v>
+        <v>-6600</v>
       </c>
     </row>
     <row r="239">
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="D242" s="1" t="n">
-        <v>-235</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="243">

</xml_diff>

<commit_message>
Addec addition script. Added error message when a Sheet is not named correctly.
</commit_message>
<xml_diff>
--- a/Lagerbestand-M0129.xlsx
+++ b/Lagerbestand-M0129.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>275</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2031</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="10">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D14" s="1" t="n">
-        <v>2008</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="15">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D15" s="1" t="n">
-        <v>240</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="D16" s="1" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="D17" s="1" t="n">
-        <v>130</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18">
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="D18" s="1" t="n">
-        <v>260</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="D19" s="1" t="n">
-        <v>662</v>
+        <v>862</v>
       </c>
     </row>
     <row r="20">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="D21" s="1" t="n">
-        <v>737</v>
+        <v>837</v>
       </c>
     </row>
     <row r="22">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D22" s="1" t="n">
-        <v>1695</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="23">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="D23" s="1" t="n">
-        <v>872</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="24">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D29" s="1" t="n">
-        <v>2889</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="30">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="D30" s="1" t="n">
-        <v>-1063</v>
+        <v>-1117</v>
       </c>
     </row>
     <row r="31">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="D33" s="1" t="n">
-        <v>-109</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="D38" s="1" t="n">
-        <v>668</v>
+        <v>868</v>
       </c>
     </row>
     <row r="39">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="D40" s="1" t="n">
-        <v>-66</v>
+        <v>-69</v>
       </c>
     </row>
     <row r="41">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="D41" s="1" t="n">
-        <v>2345</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="42">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D42" s="1" t="n">
-        <v>643</v>
+        <v>439</v>
       </c>
     </row>
     <row r="43">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="D43" s="1" t="n">
-        <v>-2160</v>
+        <v>-2316</v>
       </c>
     </row>
     <row r="44">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D45" s="1" t="n">
-        <v>2272</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="46">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="D46" s="1" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47">
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="D48" s="1" t="n">
-        <v>-20</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49">
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="D51" s="1" t="n">
-        <v>-1320</v>
+        <v>-1380</v>
       </c>
     </row>
     <row r="52">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D52" s="1" t="n">
-        <v>-32</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="53">
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="D53" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1142</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="57">
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="D63" s="1" t="n">
-        <v>-183</v>
+        <v>-198</v>
       </c>
     </row>
     <row r="64">
@@ -1546,7 +1546,7 @@
         </is>
       </c>
       <c r="D67" s="1" t="n">
-        <v>294</v>
+        <v>494</v>
       </c>
     </row>
     <row r="68">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="D74" s="1" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D75" s="1" t="n">
-        <v>-479</v>
+        <v>-524</v>
       </c>
     </row>
     <row r="76">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="D76" s="1" t="n">
-        <v>-6</v>
+        <v>-306</v>
       </c>
     </row>
     <row r="77">
@@ -1816,7 +1816,7 @@
         </is>
       </c>
       <c r="D82" s="1" t="n">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="D90" s="1" t="n">
-        <v>272</v>
+        <v>517</v>
       </c>
     </row>
     <row r="91">
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="D91" s="1" t="n">
-        <v>415</v>
+        <v>669</v>
       </c>
     </row>
     <row r="92">
@@ -1996,7 +1996,7 @@
         </is>
       </c>
       <c r="D92" s="1" t="n">
-        <v>673</v>
+        <v>933</v>
       </c>
     </row>
     <row r="93">
@@ -2014,7 +2014,7 @@
         </is>
       </c>
       <c r="D93" s="1" t="n">
-        <v>307</v>
+        <v>558</v>
       </c>
     </row>
     <row r="94">
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="D97" s="1" t="n">
-        <v>408</v>
+        <v>378</v>
       </c>
     </row>
     <row r="98">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="D99" s="1" t="n">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="D118" s="1" t="n">
-        <v>-182</v>
+        <v>-194</v>
       </c>
     </row>
     <row r="119">
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="D124" s="1" t="n">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="125">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="D125" s="1" t="n">
-        <v>-76</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="126">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="D127" s="1" t="n">
-        <v>357</v>
+        <v>514</v>
       </c>
     </row>
     <row r="128">
@@ -2644,7 +2644,7 @@
         </is>
       </c>
       <c r="D128" s="1" t="n">
-        <v>318</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129">
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="D155" s="1" t="n">
-        <v>-2358</v>
+        <v>-2658</v>
       </c>
     </row>
     <row r="156">
@@ -3220,7 +3220,7 @@
         </is>
       </c>
       <c r="D160" s="1" t="n">
-        <v>380</v>
+        <v>631</v>
       </c>
     </row>
     <row r="161">
@@ -3580,7 +3580,7 @@
         </is>
       </c>
       <c r="D180" s="1" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="D181" s="1" t="n">
-        <v>-54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -3616,7 +3616,7 @@
         </is>
       </c>
       <c r="D182" s="1" t="n">
-        <v>-132</v>
+        <v>-138</v>
       </c>
     </row>
     <row r="183">
@@ -3814,7 +3814,7 @@
         </is>
       </c>
       <c r="D193" s="1" t="n">
-        <v>22</v>
+        <v>102</v>
       </c>
     </row>
     <row r="194">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="D207" s="1" t="n">
-        <v>-6629</v>
+        <v>-6889</v>
       </c>
     </row>
     <row r="208">
@@ -4390,7 +4390,7 @@
         </is>
       </c>
       <c r="D225" s="1" t="n">
-        <v>-50</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="226">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="D230" s="1" t="n">
-        <v>-1650</v>
+        <v>-1685</v>
       </c>
     </row>
     <row r="231">
@@ -4498,7 +4498,7 @@
         </is>
       </c>
       <c r="D231" s="1" t="n">
-        <v>-26</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="232">
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="D238" s="1" t="n">
-        <v>-6600</v>
+        <v>-6900</v>
       </c>
     </row>
     <row r="239">
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="D242" s="1" t="n">
-        <v>-240</v>
+        <v>-255</v>
       </c>
     </row>
     <row r="243">
@@ -4966,7 +4966,7 @@
         </is>
       </c>
       <c r="D257" s="1" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="258">
@@ -5074,7 +5074,7 @@
         </is>
       </c>
       <c r="D263" s="1" t="n">
-        <v>151.856</v>
+        <v>191.856</v>
       </c>
     </row>
     <row r="264">
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="D266" s="1" t="n">
-        <v>260</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>